<commit_message>
Day 02: Best Time to Buy and Sell Stock — notes and solution
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://essexuniversity-my.sharepoint.com/personal/sv24670_essex_ac_uk/Documents/Leetcode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_E63E9EDDCA81E8E2DBE31B45769FC8CF512D1B66" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D809E5F-7989-4B41-AE00-E58B81AE70F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F2440D-7F37-3F40-BC38-36C4FF9583BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="342">
   <si>
     <t>Day</t>
   </si>
@@ -1050,6 +1050,21 @@
   </si>
   <si>
     <t>Algo Bonus</t>
+  </si>
+  <si>
+    <t>✅ Solved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Use HashMap to store seen numbers and their indices. For each number, compute target – num. If it exists in the map → return the two indices. Insert current number only after checking to avoid pairing with itself.
+	•	Pattern: Hashing / Complement lookup.
+	•	Edge cases: Must return indices (not values). Exactly one valid solution guaranteed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Track the minimum price so far as you scan the array. For each price, compute profit = current price – min price. Update max profit whenever this profit is greater. This ensures we always “buy” before “sell.”
+	•	Pattern: Single-pass scan with running minimum (Greedy / Prefix minimum).
+	•	Edge cases:
+	•	If prices always decrease → return 0 (no profit possible).
+	•	Must sell after buying (indices: buy &lt; sell).</t>
   </si>
 </sst>
 </file>
@@ -1119,32 +1134,29 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1446,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1462,90 +1474,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:11" ht="160" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="F2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="192" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F3" t="s">
-        <v>334</v>
+      <c r="F3" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F4" t="s">
-        <v>334</v>
-      </c>
+      <c r="F4" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="J4" t="s">
         <v>334</v>
       </c>
@@ -1554,2606 +1580,2864 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F5" t="s">
-        <v>334</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="F5" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
         <v>72</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F6" t="s">
-        <v>334</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="J6" s="1" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>97</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="J7" s="3">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>335</v>
       </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="J8" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F9" t="s">
-        <v>334</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="F9" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="J9" s="1">
         <f>COUNTIF(F2:F133,"Mock")</f>
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>336</v>
       </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F11" t="s">
-        <v>334</v>
-      </c>
+      <c r="F11" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F12" t="s">
-        <v>334</v>
-      </c>
+      <c r="F12" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F13" t="s">
-        <v>334</v>
-      </c>
+      <c r="F13" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>104</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F14" t="s">
-        <v>334</v>
-      </c>
+      <c r="F14" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F15" t="s">
-        <v>334</v>
-      </c>
+      <c r="F15" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>106</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>107</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>108</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F18" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="F18" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F20" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="F20" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F21" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="F21" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>111</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F22" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="F22" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F23" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="F23" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F24" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="F24" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>3</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>117</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F28" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="F28" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>3</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>4</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F30" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="F30" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>119</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F31" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="F31" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F32" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="F32" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>4</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F33" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="F33" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F34" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="F34" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>4</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>4</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
         <v>124</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>4</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F37" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="F37" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>4</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>5</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F39" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="F39" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>5</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="3" t="s">
         <v>127</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F40" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="F40" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>5</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>128</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F41" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="F41" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="3">
         <v>5</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>129</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F42" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="F42" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <v>5</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="3" t="s">
         <v>130</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F43" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="F43" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="3">
         <v>5</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
         <v>5</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="3" t="s">
         <v>132</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>5</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="3" t="s">
         <v>133</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="3">
         <v>5</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="3" t="s">
         <v>134</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F47" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="F47" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="3">
         <v>5</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="3">
         <v>6</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="3" t="s">
         <v>135</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="F49" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="F49" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="3">
         <v>6</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F50" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="F50" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="3">
         <v>6</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="3" t="s">
         <v>137</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F51" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="F51" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="3">
         <v>6</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="3" t="s">
         <v>138</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F52" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="F52" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="3">
         <v>6</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="3" t="s">
         <v>139</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F53" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="F53" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="3">
         <v>6</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="3" t="s">
         <v>140</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="3">
         <v>6</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="3">
         <v>6</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F56" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="F56" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="3">
         <v>6</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="3">
         <v>7</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="3" t="s">
         <v>143</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F58" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="F58" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="3">
         <v>7</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="F59" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="F59" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="3">
         <v>7</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="F60" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="F60" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="3">
         <v>7</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F61" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="F61" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="3">
         <v>7</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="F62" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="F62" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="3">
         <v>7</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="3" t="s">
         <v>148</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="3">
         <v>7</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="3" t="s">
         <v>149</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="3">
         <v>7</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="3" t="s">
         <v>150</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="3">
         <v>7</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="3" t="s">
         <v>151</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F66" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="F66" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="3">
         <v>7</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="3">
         <v>8</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F68" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="F68" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="3">
         <v>8</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="3" t="s">
         <v>153</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F69" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="F69" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="3">
         <v>8</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F70" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71">
+      <c r="F70" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="3">
         <v>8</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F71" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="F71" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="3">
         <v>8</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F72" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="F72" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="3">
         <v>8</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="3" t="s">
         <v>157</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="3">
         <v>8</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="3" t="s">
         <v>158</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
         <v>74</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="3">
         <v>8</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F75" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="F75" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="3">
         <v>8</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
         <v>76</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="3">
         <v>9</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F77" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="F77" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
         <v>77</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="3">
         <v>9</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="3" t="s">
         <v>161</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
         <v>78</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="3">
         <v>9</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="3" t="s">
         <v>162</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F79" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="F79" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="3">
         <v>9</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="3" t="s">
         <v>163</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F80" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="F80" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="3">
         <v>9</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="3">
         <v>9</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="3" t="s">
         <v>165</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F82" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="F82" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
         <v>82</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="3">
         <v>9</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="3" t="s">
         <v>166</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="3">
         <v>83</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="3">
         <v>9</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="3" t="s">
         <v>167</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F84" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="F84" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="3">
         <v>9</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="3" t="s">
         <v>168</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="3">
         <v>85</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="3">
         <v>9</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="3" t="s">
         <v>169</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87">
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="3">
         <v>86</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="3">
         <v>9</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="3" t="s">
         <v>170</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="3">
         <v>87</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="3">
         <v>9</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="3" t="s">
         <v>171</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="3">
         <v>88</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="3">
         <v>9</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="3" t="s">
         <v>172</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F89" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="F89" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="3">
         <v>89</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="3">
         <v>9</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91">
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="3">
         <v>90</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="3">
         <v>10</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="3" t="s">
         <v>173</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F91" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="F91" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="3">
         <v>91</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="3">
         <v>10</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="3" t="s">
         <v>174</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="3">
         <v>92</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="3">
         <v>10</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="3" t="s">
         <v>175</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F93" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="F93" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
         <v>93</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="3">
         <v>10</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="3" t="s">
         <v>176</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
         <v>94</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="3">
         <v>10</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F95" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="F95" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
         <v>95</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="3">
         <v>10</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="3" t="s">
         <v>178</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="3">
         <v>96</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="3">
         <v>10</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F97" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="F97" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="3">
         <v>97</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="3">
         <v>10</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="3" t="s">
         <v>180</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="3">
         <v>98</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="3">
         <v>10</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="3" t="s">
         <v>181</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F99" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100">
+      <c r="F99" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="3">
         <v>99</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="3">
         <v>10</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="3" t="s">
         <v>182</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="3">
         <v>100</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="3">
         <v>10</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="3" t="s">
         <v>183</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102">
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
         <v>101</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="3">
         <v>10</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103">
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="3">
         <v>102</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="3">
         <v>10</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="3" t="s">
         <v>185</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104">
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="3">
         <v>103</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="3">
         <v>10</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="3" t="s">
         <v>186</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F104" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105">
+      <c r="F104" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="3">
         <v>104</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="3">
         <v>10</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F105" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106">
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="3">
         <v>105</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="3">
         <v>11</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="3" t="s">
         <v>187</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F106" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107">
+      <c r="F106" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
         <v>106</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="3">
         <v>11</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="3" t="s">
         <v>188</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108">
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
         <v>107</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="3">
         <v>11</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F108" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109">
+      <c r="F108" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
         <v>108</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="3">
         <v>11</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="3" t="s">
         <v>190</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F109" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110">
+      <c r="F109" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
         <v>109</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="3">
         <v>11</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="3" t="s">
         <v>191</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F110" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111">
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
         <v>110</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="3">
         <v>11</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="3" t="s">
         <v>192</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F111" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112">
+      <c r="F111" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
         <v>111</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="3">
         <v>11</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="3" t="s">
         <v>193</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113">
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
         <v>112</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="3">
         <v>11</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="3" t="s">
         <v>194</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F113" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114">
+      <c r="F113" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
         <v>113</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="3">
         <v>11</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="3" t="s">
         <v>195</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F114" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115">
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
         <v>114</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="3">
         <v>11</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="3" t="s">
         <v>196</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F115" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116">
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
         <v>115</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="3">
         <v>11</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="3" t="s">
         <v>197</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F116" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117">
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
         <v>116</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="3">
         <v>11</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="3" t="s">
         <v>198</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F117" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118">
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
         <v>117</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="3">
         <v>11</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="3" t="s">
         <v>199</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F118" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119">
+      <c r="F118" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
         <v>118</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="3">
         <v>11</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120">
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
         <v>119</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="3">
         <v>12</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="3" t="s">
         <v>200</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F120" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121">
+      <c r="F120" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
         <v>120</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="3">
         <v>12</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="3" t="s">
         <v>201</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F121" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122">
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
         <v>121</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="3">
         <v>12</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="3" t="s">
         <v>202</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F122" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123">
+      <c r="F122" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
         <v>122</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="3">
         <v>12</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="3" t="s">
         <v>203</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F123" t="s">
+      <c r="F123" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124">
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
         <v>123</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="3">
         <v>12</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="3" t="s">
         <v>204</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="F124" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125">
+      <c r="F124" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
         <v>124</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="3">
         <v>12</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="3" t="s">
         <v>205</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F125" t="s">
+      <c r="F125" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126">
+      <c r="G125" s="3"/>
+      <c r="H125" s="3"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
         <v>125</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="3">
         <v>12</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="3" t="s">
         <v>206</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F126" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127">
+      <c r="F126" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
         <v>126</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="3">
         <v>12</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="3" t="s">
         <v>207</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F127" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128">
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
         <v>127</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="3">
         <v>12</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="3" t="s">
         <v>208</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F128" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129">
+      <c r="F128" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G128" s="3"/>
+      <c r="H128" s="3"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
         <v>128</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="3">
         <v>12</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="3" t="s">
         <v>209</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130">
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
         <v>129</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="3">
         <v>12</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="3" t="s">
         <v>210</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F130" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131">
+      <c r="G130" s="3"/>
+      <c r="H130" s="3"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
         <v>130</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="3">
         <v>12</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="3" t="s">
         <v>211</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F131" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132">
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
         <v>131</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="3">
         <v>12</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="3" t="s">
         <v>212</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="F132" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133">
+      <c r="F132" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
         <v>132</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="3">
         <v>12</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F133" s="3" t="s">
         <v>336</v>
       </c>
+      <c r="G133" s="3"/>
+      <c r="H133" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B133">
@@ -4170,7 +4454,19 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F133">
+  <conditionalFormatting sqref="F2:F133 G2:G3 H3">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{01133F43-9E31-5643-91E7-C222DF1503F0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -4180,18 +4476,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{A23B4E13-A755-BE44-B4B4-33678A2E9C98}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{01133F43-9E31-5643-91E7-C222DF1503F0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4348,6 +4632,14 @@
           <xm:sqref>B2:B133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{01133F43-9E31-5643-91E7-C222DF1503F0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
           <x14:cfRule type="dataBar" id="{A23B4E13-A755-BE44-B4B4-33678A2E9C98}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
@@ -4356,15 +4648,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{01133F43-9E31-5643-91E7-C222DF1503F0}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F2:F133</xm:sqref>
+          <xm:sqref>F2:F133 G2:G3 H3</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Day 03: Valid Anagram - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F2440D-7F37-3F40-BC38-36C4FF9583BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B10CA07-C244-1241-9908-2098396836D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="346">
   <si>
     <t>Day</t>
   </si>
@@ -1066,12 +1066,31 @@
 	•	If prices always decrease → return 0 (no profit possible).
 	•	Must sell after buying (indices: buy &lt; sell).</t>
   </si>
+  <si>
+    <t>Algo(Hashmap / String)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach:
+Use a HashMap (or Python Counter) to count character frequencies of both strings. First, check if their lengths differ — if yes, immediately return False. Then compare the two frequency maps; if they match, return True. This ensures both strings contain the same characters with the same counts.
+	•	Pattern:
+Hashmap frequency counting. Can also solve by sorting both strings and comparing, but that’s slower (O(n log n)).
+	•	Edge cases:
+	•	Strings with same characters but different counts (e.g., "aab" vs "ab") → must return False.
+	•	Length mismatch → immediate False.
+	•	If extended to Unicode, need a more general counting approach.</t>
+  </si>
+  <si>
+    <t>Algo(Array, (DP)Dynamic Programming (one-pass optimization))</t>
+  </si>
+  <si>
+    <t>Algo(Array, Hashmap )</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1093,6 +1112,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1118,9 +1145,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1134,7 +1159,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1145,18 +1170,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1167,6 +1265,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CAB5B45-EC52-AE4B-8EB8-4353E1384E2D}" name="Table2" displayName="Table2" ref="A1:H133" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H133" xr:uid="{1CAB5B45-EC52-AE4B-8EB8-4353E1384E2D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{E9A8D136-B3CC-9B46-BAC7-E5F77E502E4D}" name="Day" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{FB70F782-0BD7-4941-9476-3E5649457B69}" name="Week" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{A3A502B3-C39F-7F4D-A54B-8BD14E512A08}" name="Date" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{7BEBA866-C507-5C4F-B4AD-F403A414AF1A}" name="Problem" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{55E3BBDA-3A64-4045-B047-976D690CE368}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{D5F10497-9C64-6646-A803-9234F5E03A28}" name="Category" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{0D300B93-0B8F-6743-B360-584EAAF1D0D5}" name="Status (✅/❌)" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{7A995E53-0648-BF4C-B371-BAC211FABE7F}" name="Notes" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1458,44 +1573,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="5" width="63.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="35.83203125" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1516,12 +1632,12 @@
         <v>213</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>340</v>
       </c>
     </row>
@@ -1542,16 +1658,16 @@
         <v>214</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="304" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1568,10 +1684,14 @@
         <v>215</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+        <v>342</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>343</v>
+      </c>
       <c r="J4" t="s">
         <v>334</v>
       </c>
@@ -1602,7 +1722,7 @@
       <c r="H5" s="3"/>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -4454,8 +4574,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F133 G2:G3 H3">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="G2:G4 F2:F133 H3:H4">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4467,7 +4587,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4615,6 +4735,9 @@
     <hyperlink ref="E133" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId133"/>
+  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -4648,7 +4771,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F133 G2:G3 H3</xm:sqref>
+          <xm:sqref>G2:G4 F2:F133 H3:H4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Day 04: Contains Duplicate  - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B10CA07-C244-1241-9908-2098396836D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED77CC1E-0B27-0E4A-9429-6CF276242718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="348">
   <si>
     <t>Day</t>
   </si>
@@ -1084,6 +1084,19 @@
   </si>
   <si>
     <t>Algo(Array, Hashmap )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach:
+Use a HashSet to track numbers seen so far. Iterate through the array; for each number, check if it already exists in the set. If yes → return True (duplicate found). Otherwise, add the number to the set. If the loop ends without finding duplicates → return False.
+	•	Pattern:
+Hashing / Duplicate detection. Alternative solution is to sort the array and check adjacent elements, but that takes O(n log n) instead of O(n).
+	•	Edge cases:
+	•	Empty array → should return False (no duplicates).
+	•	Single element → should return False.
+	•	Large arrays (up to 10⁵ elements) must still run efficiently in O(n).</t>
+  </si>
+  <si>
+    <t>Algo(Array / Hashset)</t>
   </si>
 </sst>
 </file>
@@ -1573,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1699,7 +1712,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="288" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1716,13 +1729,17 @@
         <v>216</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+        <v>347</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -4574,7 +4591,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4 F2:F133 H3:H4">
+  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G5">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -4771,7 +4788,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G2:G4 F2:F133 H3:H4</xm:sqref>
+          <xm:sqref>F2:F133 H3:H4 G2:G5</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Day 05: Binary Search - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED77CC1E-0B27-0E4A-9429-6CF276242718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D3FB0C-7D9A-7241-9DC1-242877BC10EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="350">
   <si>
     <t>Day</t>
   </si>
@@ -1097,6 +1097,19 @@
   </si>
   <si>
     <t>Algo(Array / Hashset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach:
+Use Binary Search on the sorted array. Maintain left and right pointers. At each step, compute mid = (left + right) // 2. Compare nums[mid] with target: if equal → return index; if smaller → move left; if larger → move right. Continue until left &gt; right.
+	•	Pattern:
+Binary Search / Divide and Conquer.
+	•	Edge cases:
+	•	Single element array (either return 0 or -1).
+	•	Target not found → must return -1.
+	•	Watch out for infinite loops (always update left or right).</t>
+  </si>
+  <si>
+    <t>Algo(Array / Binary Search)</t>
   </si>
 </sst>
 </file>
@@ -1586,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,14 +1752,14 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="224" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1763,10 +1776,14 @@
         <v>217</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <v>349</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="J6" s="1" t="s">
         <v>335</v>
       </c>
@@ -4591,7 +4608,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G5">
+  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G6">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -4788,7 +4805,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F133 H3:H4 G2:G5</xm:sqref>
+          <xm:sqref>F2:F133 H3:H4 G2:G6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Day 06: Customers Who Never Order (SQL) — solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D3FB0C-7D9A-7241-9DC1-242877BC10EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77174F8-53C5-BB4D-B16D-5305D972431A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="354">
   <si>
     <t>Day</t>
   </si>
@@ -1110,6 +1110,31 @@
   </si>
   <si>
     <t>Algo(Array / Binary Search)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Use LEFT JOIN between Person and Address on personId. Select firstName, lastName, city, state. Ensures all persons are included even if they don’t have an address (NULL values fill missing).
+	•	Pattern: SQL Joins → specifically LEFT JOIN for optional relationships.
+	•	Edge cases:
+	•	Person without an address → city/state should return NULL.
+	•	If we mistakenly use INNER JOIN, those rows would be excluded.
+	•	Works regardless of address table having extra unmatched rows.</t>
+  </si>
+  <si>
+    <t>SQL / JOINs</t>
+  </si>
+  <si>
+    <t>Approach:
+Use a LEFT JOIN between Customers and Orders on id = customerId. Keep only rows where Orders.customerId is NULL → these are customers with no orders. Alternative: NOT EXISTS subquery.
+Pattern:
+SQL Anti-join (LEFT JOIN … IS NULL) / NOT EXISTS.
+Complexity:
+Efficient with proper indexes on Customers(id) and Orders(customerId).
+Edge cases:
+	•	Customers table can include people with no matching record in Orders → must appear in result.
+	•	Be cautious using NOT IN if subquery has NULL values (engine-dependent).</t>
+  </si>
+  <si>
+    <t>SQL / Anti-join</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1788,7 +1813,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="224" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1805,16 +1830,20 @@
         <v>218</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>351</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1831,10 +1860,14 @@
         <v>219</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+        <v>353</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>352</v>
+      </c>
       <c r="J8" t="s">
         <v>336</v>
       </c>
@@ -4608,7 +4641,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G6">
+  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G8">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -4805,7 +4838,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F133 H3:H4 G2:G6</xm:sqref>
+          <xm:sqref>F2:F133 H3:H4 G2:G8</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Day 07: Intersection of Two Arrays II — solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E501C4D-AA98-5843-A85B-C6A278D789C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0F42F1-2C3D-AB41-986E-05B4BCD9FCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="357">
   <si>
     <t>Day</t>
   </si>
@@ -1135,6 +1135,21 @@
   </si>
   <si>
     <t>SQL / Anti-join</t>
+  </si>
+  <si>
+    <t>✅ Solved(</t>
+  </si>
+  <si>
+    <t>Algo(Array / Hashmap  (Alt: Two Pointers if arrays are sorted))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Use a frequency map (Counter) for the smaller array. For each element in the other array, if its count &gt; 0, include it in the result and decrement the count. This ensures duplicates are counted correctly.
+	•	Pattern: Hashmap frequency counting (alternative: Two Pointers if arrays are already sorted).
+	•	Complexity: Time O(n + m), Space O(min(n, m)).
+	•	Edge Cases:
+	•	No overlap → result is empty list [].
+	•	Handles duplicates correctly (min count from both arrays).
+	•	If one array is huge and stored externally, process the smaller in memory, stream through the larger.</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1777,7 +1792,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -1863,7 +1878,7 @@
         <v>353</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>352</v>
@@ -1872,7 +1887,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1889,10 +1904,14 @@
         <v>220</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+        <v>355</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>356</v>
+      </c>
       <c r="J9" s="1">
         <f>COUNTIF(F2:F133,"Mock")</f>
         <v>12</v>
@@ -4641,7 +4660,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G8">
+  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G9">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -4838,7 +4857,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F133 H3:H4 G2:G8</xm:sqref>
+          <xm:sqref>F2:F133 H3:H4 G2:G9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
ay 08: Maximum Subarray - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0F42F1-2C3D-AB41-986E-05B4BCD9FCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39641486-F76B-DD4F-BCAD-BF06167AAB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1639,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Day 09: Move Zeroes - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39641486-F76B-DD4F-BCAD-BF06167AAB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C52A91-FB64-2649-9ABC-C928D6E17380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="361">
   <si>
     <t>Day</t>
   </si>
@@ -1150,6 +1150,46 @@
 	•	No overlap → result is empty list [].
 	•	Handles duplicates correctly (min count from both arrays).
 	•	If one array is huge and stored externally, process the smaller in memory, stream through the larger.</t>
+  </si>
+  <si>
+    <t>Algo(Array / Dynamic Programming (Kadane), (Alt) Divide &amp; Conquer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach:
+Use Kadane’s Algorithm. Maintain two variables:
+	•	curr_sum = maximum subarray sum ending at the current index.
+	•	max_sum = global maximum found so far.
+At each step:
+curr_sum = max(nums[i], curr_sum + nums[i])
+max_sum = max(max_sum, curr_sum)
+This ensures that if adding the current number reduces the sum, we “restart” the subarray at that index.
+Divide &amp; Conquer is another valid approach (O(n log n)), but Kadane’s is more efficient.
+	•	Pattern:
+Dynamic Programming (1D DP) / Running sum reset.
+Related problems: Maximum Circular Subarray, Best Time to Buy and Sell Stock, Maximum Product Subarray.
+	•	Complexity:
+	•	Time: O(n) (one pass through array)
+	•	Space: O(1) (just two variables)
+	•	Edge Cases:
+	•	All negative numbers → return the maximum single element.
+	•	Single-element array → return that element.
+	•	Mix of positives and negatives → handled naturally.
+	•	Notes:
+	•	Don’t initialize curr_sum = 0, or all-negative arrays will break.
+	•	Correct initialization: curr_sum = max_sum = nums[0].
+	•	Kadane’s algorithm is essentially a greedy + DP hybrid.</t>
+  </si>
+  <si>
+    <t>Algo(Array / Two Pointers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Use two pointers. Keep a pos pointer for the next non-zero placement. Iterate through nums; whenever a non-zero is found, place it at nums[pos] and increment pos. After the pass, fill remaining indices with zeros.
+	•	Pattern: Two Pointers (read/write), In-place array modification.
+	•	Complexity: Time O(n), Space O(1).
+	•	Edge cases:
+	•	All zeros → array unchanged.
+	•	No zeros → array unchanged.
+	•	Mixed zeros and non-zeros → must preserve relative order of non-zeros.</t>
   </si>
 </sst>
 </file>
@@ -1639,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1792,7 +1832,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -1939,7 +1979,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1956,12 +1996,16 @@
         <v>222</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="224" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1978,10 +2022,14 @@
         <v>223</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+        <v>359</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3">

</xml_diff>

<commit_message>
Day 10: Merge Sorted Array — solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C52A91-FB64-2649-9ABC-C928D6E17380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7E5FB3-621E-B748-B18A-8FD266B27513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="363">
   <si>
     <t>Day</t>
   </si>
@@ -1190,6 +1190,15 @@
 	•	All zeros → array unchanged.
 	•	No zeros → array unchanged.
 	•	Mixed zeros and non-zeros → must preserve relative order of non-zeros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Two pointers from the end. Use i=m-1, j=n-1, k=m+n-1. Write the larger of nums1[i]/nums2[j] to nums1[k], move pointers. Copy remaining nums2 if any.
+	•	Pattern: Two Pointers (in-place, from end).
+	•	Complexity: Time O(m+n), Space O(1).
+	•	Edge cases: m=0 (all from nums2), n=0 (nums1 unchanged), interleaved values.</t>
+  </si>
+  <si>
+    <t>Algo(Array / Two Pointers (from the end))</t>
   </si>
 </sst>
 </file>
@@ -1679,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1832,7 +1841,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2031,7 +2040,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="128" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2048,10 +2057,14 @@
         <v>224</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+        <v>362</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -4708,7 +4721,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F133 H3:H4 G2:G9">
+  <conditionalFormatting sqref="H3:H4 G2:G9 F2:F133">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -4905,7 +4918,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F133 H3:H4 G2:G9</xm:sqref>
+          <xm:sqref>H3:H4 G2:G9 F2:F133</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Day 11: Valid Palindrome - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77371C9A-C9EA-DC45-B858-8EABF913194C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99054912-C2F3-A44F-B1D3-CFB99A88217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="365">
   <si>
     <t>Day</t>
   </si>
@@ -1202,6 +1202,15 @@
 	•	m = 0 → all elements come from nums2.
 	•	n = 0 → nums1 remains unchanged.
 	•	Already sorted arrays → merge loop still works correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Normalize string by converting to lowercase and removing non-alphanumeric characters. Then compare with its reverse (or use two pointers).
+	•	Complexity: Time O(n), Space O(n) (O(1) if two-pointer).
+	•	Patterns: Two Pointers, String normalization.
+	•	Notes: Empty string is valid palindrome; must ignore cases and symbols; regex helps simplify filtering.</t>
+  </si>
+  <si>
+    <t>Algo(String / Two Pointers)</t>
   </si>
 </sst>
 </file>
@@ -1691,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1844,7 +1853,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2069,7 +2078,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2086,10 +2095,14 @@
         <v>225</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+        <v>364</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3">

</xml_diff>

<commit_message>
Day 12: Climbing Stairs - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99054912-C2F3-A44F-B1D3-CFB99A88217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0751597-51CD-DA4A-8CA3-B0E2480F1FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="367">
   <si>
     <t>Day</t>
   </si>
@@ -1211,6 +1211,22 @@
   </si>
   <si>
     <t>Algo(String / Two Pointers)</t>
+  </si>
+  <si>
+    <t>Algo(Dynamic Programming)</t>
+  </si>
+  <si>
+    <t>Approach:
+Use Dynamic Programming with the recurrence dp[n] = dp[n-1] + dp[n-2]. Optimize with two variables (prev1, prev2) instead of an array.
+Pattern:
+Dynamic Programming (Fibonacci-like recurrence).
+Complexity:
+Time: O(n), Space: O(1).
+Notes:
+	•	Base cases: n=1 → 1, n=2 → 2.
+	•	Key insight: ways to reach step n = sum of ways to (n-1) and (n-2).
+	•	Optimize DP storage to O(1).
+	•	Related: Min Cost Climbing Stairs, House Robber.</t>
   </si>
 </sst>
 </file>
@@ -1700,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1853,7 +1869,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2104,7 +2120,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="320" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2121,10 +2137,14 @@
         <v>226</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+        <v>365</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3">

</xml_diff>

<commit_message>
Day 13: Department Highest Salary (SQL) — solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0751597-51CD-DA4A-8CA3-B0E2480F1FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BF3C0C-314D-5244-9014-0D6DFA073345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="369">
   <si>
     <t>Day</t>
   </si>
@@ -1227,6 +1227,15 @@
 	•	Key insight: ways to reach step n = sum of ways to (n-1) and (n-2).
 	•	Optimize DP storage to O(1).
 	•	Related: Min Cost Climbing Stairs, House Robber.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Use RANK() OVER (PARTITION BY departmentId ORDER BY salary DESC) and keep rows where rank = 1; join to Department for names.
+	•	Pattern: Window functions (Top-N per group). Alt: MAX(salary) per department + join.
+	•	Complexity: Good with indexes on (departmentId, salary).
+	•	Edge cases: Multiple employees can tie for top salary → RANK() includes all.</t>
+  </si>
+  <si>
+    <t>SQL(Window Functions (ALT: Aggregation + Join))</t>
   </si>
 </sst>
 </file>
@@ -1716,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1932,7 +1941,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -2146,7 +2155,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2163,10 +2172,14 @@
         <v>227</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+        <v>368</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3">

</xml_diff>

<commit_message>
Day 13: Second Highest Salary (SQL) — solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BF3C0C-314D-5244-9014-0D6DFA073345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB61328-DE8E-5746-8D5D-990A8A28B621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="371">
   <si>
     <t>Day</t>
   </si>
@@ -1236,6 +1236,15 @@
   </si>
   <si>
     <t>SQL(Window Functions (ALT: Aggregation + Join))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Rank salaries with DENSE_RANK() descending, pick where rank = 2. Or use DISTINCT salary ORDER BY DESC LIMIT 1 OFFSET 1.
+	•	Pattern: Window function ranking / Top-K query.
+	•	Complexity: O(n log n) due to sorting.
+	•	Edge cases: If only one distinct salary exists, return NULL.</t>
+  </si>
+  <si>
+    <t>SQL(Window Functions (ALT: Subquery with DISTINCT))</t>
   </si>
 </sst>
 </file>
@@ -1725,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1941,7 +1950,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -2181,7 +2190,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2198,10 +2207,14 @@
         <v>228</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+        <v>370</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3">

</xml_diff>

<commit_message>
Day 14: Search Insert Position - binary search solution + notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB61328-DE8E-5746-8D5D-990A8A28B621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24396E37-8DA8-8F4A-9292-16341433A2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="373">
   <si>
     <t>Day</t>
   </si>
@@ -1245,6 +1245,22 @@
   </si>
   <si>
     <t>SQL(Window Functions (ALT: Subquery with DISTINCT))</t>
+  </si>
+  <si>
+    <t>Approach:
+Use Binary Search to locate the target. If found, return its index. If not, return the index where it should be inserted in order. After the loop, the left pointer indicates the correct insert position.
+Pattern:
+Binary Search (Divide &amp; Conquer).
+Complexity:
+Time: O(log n), Space: O(1).
+Notes:
+	•	If target &lt; smallest element → return 0.
+	•	If target &gt; largest element → return len(nums).
+	•	left at the end always gives the right position (whether found or insert).
+	•	Related problems: First Bad Version, Search Range.</t>
+  </si>
+  <si>
+    <t>Algo(Binary Search / Array )</t>
   </si>
 </sst>
 </file>
@@ -1734,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1887,7 +1903,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2216,7 +2232,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="335" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2233,10 +2249,14 @@
         <v>229</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+        <v>372</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3">

</xml_diff>

<commit_message>
Day 15: Group Anagrams - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24396E37-8DA8-8F4A-9292-16341433A2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93A23C2-450A-3149-932B-66B6CC0249A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="374">
   <si>
     <t>Day</t>
   </si>
@@ -1261,6 +1261,12 @@
   </si>
   <si>
     <t>Algo(Binary Search / Array )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Hashmap bucketing via a canonical key. Recommended: 26-length letter-count tuple as key (O(N·L)); alternative: sorted string as key (O(N·L log L)).
+	•	Pattern: Hashmap grouping; canonical representation for anagrams.
+	•	Complexity: Time O(N·L) (count signature) or O(N·L log L) (sorted); Space O(N·L).
+	•	Notes: Handles empty strings and duplicates. Order of groups/elements doesn’t matter.</t>
   </si>
 </sst>
 </file>
@@ -1750,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1903,7 +1909,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2280,7 +2286,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2297,10 +2303,14 @@
         <v>230</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+        <v>342</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3">

</xml_diff>

<commit_message>
Day 16: Subarray Sum Equals K - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93A23C2-450A-3149-932B-66B6CC0249A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D10D85-A709-174E-ADEE-FC41B6F95A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="376">
   <si>
     <t>Day</t>
   </si>
@@ -1267,6 +1267,15 @@
 	•	Pattern: Hashmap grouping; canonical representation for anagrams.
 	•	Complexity: Time O(N·L) (count signature) or O(N·L log L) (sorted); Space O(N·L).
 	•	Notes: Handles empty strings and duplicates. Order of groups/elements doesn’t matter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Prefix Sum + HashMap. Maintain counts of seen prefix sums. For each index, add count[prefix - k] to total, then increment count[prefix]. Initialize count[0] = 1 to count subarrays starting at index 0.
+	•	Pattern: Prefix Sum with frequency map.
+	•	Complexity: Time O(n), Space O(n).
+	•	Notes: Handles negatives/zeros; sliding window doesn’t work here. Key detail: count[0] = 1. Related: Subarray Sums Divisible by K, Path Sum III.</t>
+  </si>
+  <si>
+    <t>Algo(Array / Hashmap / Prefix Sum)</t>
   </si>
 </sst>
 </file>
@@ -1756,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1909,7 +1918,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2312,7 +2321,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2329,10 +2338,14 @@
         <v>231</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+        <v>375</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3">

</xml_diff>

<commit_message>
Day 17: Longest Substring Without Repeating Characters - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D10D85-A709-174E-ADEE-FC41B6F95A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD91392-0929-B945-AB40-CE84E03AAEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="378">
   <si>
     <t>Day</t>
   </si>
@@ -1276,6 +1276,15 @@
   </si>
   <si>
     <t>Algo(Array / Hashmap / Prefix Sum)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Sliding window with left/right and last_seen map. If s[right] was seen at index ≥ left, move left = last_seen[s[right]] + 1; update last_seen and track best = max(best, right-left+1).
+	•	Pattern: Sliding Window + HashMap.
+	•	Complexity: Time O(n), Space O(min(n, charset)).
+	•	Notes: Handles all characters (letters, digits, symbols). Move left only forward; use last index to skip past duplicates. Related: Min Window Substring, Longest Replacing K.</t>
+  </si>
+  <si>
+    <t>Algo(String / Sliding Window / HashMap)</t>
   </si>
 </sst>
 </file>
@@ -1765,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1918,7 +1927,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2347,7 +2356,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2364,10 +2373,14 @@
         <v>232</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+        <v>377</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3">

</xml_diff>

<commit_message>
Day 18: Squares of a Sorted Array - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD91392-0929-B945-AB40-CE84E03AAEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B9D90E-BFF4-3541-9BC6-8AF0F34D2000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="500" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="379">
   <si>
     <t>Day</t>
   </si>
@@ -1285,6 +1285,15 @@
   </si>
   <si>
     <t>Algo(String / Sliding Window / HashMap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Two pointers. Compare absolute values at both ends; square the larger one and fill result from back to front.
+	•	Pattern: Two Pointers (meeting from both ends).
+	•	Complexity: Time O(n), Space O(n).
+	•	Notes:
+	•	Squaring + sorting is slower (O(n log n)).
+	•	Works for negatives and positives.
+	•	Edge cases: all negative, all positive, single element.</t>
   </si>
 </sst>
 </file>
@@ -1774,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1927,7 +1936,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2382,7 +2391,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2399,10 +2408,14 @@
         <v>233</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+        <v>359</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3">

</xml_diff>

<commit_message>
Day 18: Squares of a Sorted Array - added both O(n log n) and O(n) solutions with notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B9D90E-BFF4-3541-9BC6-8AF0F34D2000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B033A-6118-4343-84ED-86FF048D4855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1287,12 +1287,14 @@
     <t>Algo(String / Sliding Window / HashMap)</t>
   </si>
   <si>
-    <t xml:space="preserve">	•	Approach: Two pointers. Compare absolute values at both ends; square the larger one and fill result from back to front.
-	•	Pattern: Two Pointers (meeting from both ends).
+    <t xml:space="preserve">	•	Approach:
+	•	Approach 1: Square then sort (O(n log n)).
+	•	Approach 2: Two pointers → compare abs(left) vs abs(right), fill result backwards (O(n)).
+	•	Pattern: Two Pointers / Array.
 	•	Complexity: Time O(n), Space O(n).
 	•	Notes:
-	•	Squaring + sorting is slower (O(n log n)).
-	•	Works for negatives and positives.
+	•	Squaring changes order when negatives are present.
+	•	Two-pointer solution avoids sorting → optimal.
 	•	Edge cases: all negative, all positive, single element.</t>
   </si>
 </sst>
@@ -1783,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2391,7 +2393,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Day 19: Find Minimum in Rotated Sorted Array - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B033A-6118-4343-84ED-86FF048D4855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5404FD-216B-A546-A8CC-42E7FE1586CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="381">
   <si>
     <t>Day</t>
   </si>
@@ -1296,6 +1296,15 @@
 	•	Squaring changes order when negatives are present.
 	•	Two-pointer solution avoids sorting → optimal.
 	•	Edge cases: all negative, all positive, single element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Binary Search. Compare nums[mid] with nums[right]. If nums[mid] &gt; nums[right], min is in right half (left = mid + 1); else min is in left half including mid (right = mid). Return nums[left].
+	•	Pattern: Rotated array + binary search.
+	•	Complexity: Time O(log n), Space O(1).
+	•	Notes: Distinct elements only. Comparing to right simplifies logic. Related: Search in Rotated Array, Find Min II (with duplicates).</t>
+  </si>
+  <si>
+    <t>Algo(Binary Search / Array)</t>
   </si>
 </sst>
 </file>
@@ -1785,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1938,7 +1947,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2419,7 +2428,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2436,10 +2445,14 @@
         <v>234</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+        <v>380</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3">

</xml_diff>

<commit_message>
Day 20: Employee Bonus - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5404FD-216B-A546-A8CC-42E7FE1586CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BD63D2-A5F5-ED44-AD5E-A4E7E56ECC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="383">
   <si>
     <t>Day</t>
   </si>
@@ -1305,6 +1305,15 @@
   </si>
   <si>
     <t>Algo(Binary Search / Array)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: LEFT JOIN Employee→Bonus; filter where bonus &lt; 1000 or bonus IS NULL.
+	•	Pattern: Outer join + conditional filter.
+	•	Complexity: Typically O(N) with indexes.
+	•	Notes: Ensures employees with no bonus record are included; excludes bonus = 1000.</t>
+  </si>
+  <si>
+    <t>SQL / Joins</t>
   </si>
 </sst>
 </file>
@@ -1794,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2010,7 +2019,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -2454,7 +2463,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2471,10 +2480,14 @@
         <v>235</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+        <v>382</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3">

</xml_diff>

<commit_message>
Day 20 Rising Temperature - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BD63D2-A5F5-ED44-AD5E-A4E7E56ECC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0599D2-B2D7-6B45-9722-0D85F7E6B501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="385">
   <si>
     <t>Day</t>
   </si>
@@ -1314,6 +1314,15 @@
   </si>
   <si>
     <t>SQL / Joins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Compare each day to exact yesterday. Option A: LAG(temp/date) + filter DATEDIFF=1 and temp &gt; prev_temp. Option B: self-join where DATEDIFF(recordDate, prevDate)=1 and w1.temp &gt; w0.temp.
+	•	Pattern: Time-series, window function vs self-join.
+	•	Complexity: Sort-based, ~O(N log N); faster with INDEX(recordDate).
+	•	Notes: Enforce exact previous day; equal temps not included; gaps are ignored.</t>
+  </si>
+  <si>
+    <t>SQL / Joins / Window Functions</t>
   </si>
 </sst>
 </file>
@@ -1803,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2019,7 +2028,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -2489,7 +2498,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2506,10 +2515,14 @@
         <v>236</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+        <v>384</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3">

</xml_diff>

<commit_message>
Day 20: Sales Person - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0599D2-B2D7-6B45-9722-0D85F7E6B501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FB9F4C-1666-4744-9A27-CA92AB2E0727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="387">
   <si>
     <t>Day</t>
   </si>
@@ -1323,6 +1323,15 @@
   </si>
   <si>
     <t>SQL / Joins / Window Functions</t>
+  </si>
+  <si>
+    <t>SQL / Joins / Filtering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Select salespersons whose sales_id does not appear in orders tied to company RED. Use NOT IN (simple) or NOT EXISTS (NULL-safe).
+	•	Pattern: Anti-join, subquery filtering.
+	•	Complexity: O(N) joins, optimized with indexes.
+	•	Notes: Must exclude only those linked to company “RED”. Others remain even if they sold to different companies.</t>
   </si>
 </sst>
 </file>
@@ -1812,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2028,7 +2037,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -2524,7 +2533,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2541,10 +2550,14 @@
         <v>237</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+        <v>385</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3">

</xml_diff>

<commit_message>
Day 21: Majority Element - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FB9F4C-1666-4744-9A27-CA92AB2E0727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D298E-3633-D84E-B21E-E84EE4A00E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="389">
   <si>
     <t>Day</t>
   </si>
@@ -1332,6 +1332,15 @@
 	•	Pattern: Anti-join, subquery filtering.
 	•	Complexity: O(N) joins, optimized with indexes.
 	•	Notes: Must exclude only those linked to company “RED”. Others remain even if they sold to different companies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Boyer–Moore Majority Vote — keep candidate, count; when count==0, set new candidate; increment if same, decrement otherwise; final candidate is majority.
+	•	Pattern: Majority Vote / Greedy cancellation.
+	•	Complexity: Time O(n), Space O(1).
+	•	Notes: Majority guaranteed by problem; Counter solution is easier but uses O(n) space; related: Majority Element II.</t>
+  </si>
+  <si>
+    <t>Algo(Array / Hashmap / Boyer–Moore Majority Vote)</t>
   </si>
 </sst>
 </file>
@@ -1821,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1974,7 +1983,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2559,7 +2568,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2576,10 +2585,14 @@
         <v>238</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+        <v>388</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3">

</xml_diff>

<commit_message>
Day 22: Valid Parentheses - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D298E-3633-D84E-B21E-E84EE4A00E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC01FE-4FE4-294A-AC07-EC4756E9600B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="391">
   <si>
     <t>Day</t>
   </si>
@@ -1341,6 +1341,22 @@
   </si>
   <si>
     <t>Algo(Array / Hashmap / Boyer–Moore Majority Vote)</t>
+  </si>
+  <si>
+    <t>🧾 Excel Tracker Notes
+Approach:
+Use a Stack to store opening brackets. For each closing bracket, verify it matches the last opening bracket on top of the stack. If mismatch or missing → return False. At the end, stack must be empty.
+Pattern:
+Stack-based matching.
+Complexity:
+Time O(n), Space O(n).
+Notes:
+	•	Check for early mismatches.
+	•	Ensure stack empty at end for validity.
+	•	Related → Balanced parentheses / expression validation.</t>
+  </si>
+  <si>
+    <t>Algo(Stack / String)</t>
   </si>
 </sst>
 </file>
@@ -1830,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1983,7 +1999,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2616,7 +2632,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="320" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2633,10 +2649,14 @@
         <v>239</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+        <v>390</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3">

</xml_diff>

<commit_message>
Day 23: Implement Queue using Stacks - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC01FE-4FE4-294A-AC07-EC4756E9600B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE447461-D6F9-E646-9C90-62E3CFD9A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="393">
   <si>
     <t>Day</t>
   </si>
@@ -1357,6 +1357,23 @@
   </si>
   <si>
     <t>Algo(Stack / String)</t>
+  </si>
+  <si>
+    <t>Approach:
+Use two stacks: in_stack (for pushing) and out_stack (for popping/peeking).
+When out_stack is empty, move all elements from in_stack → out_stack.
+This reverses order and simulates FIFO queue behavior.
+Pattern:
+Stack → Queue Simulation.
+Amortized O(1) per operation.
+Complexity:
+Time O(1) (amortized), Space O(n).
+Notes:
+	•	Move only when necessary to keep O(1) amortized.
+	•	Common interview test of stack/queue fundamentals.</t>
+  </si>
+  <si>
+    <t>Algo(Stack / Queue Simulation )</t>
   </si>
 </sst>
 </file>
@@ -1846,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1999,7 +2016,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2658,7 +2675,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="320" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2675,10 +2692,14 @@
         <v>240</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+        <v>392</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3">

</xml_diff>

<commit_message>
Day 24: Min Stack - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE447461-D6F9-E646-9C90-62E3CFD9A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B73B4F-7637-D749-828E-E4A899153877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="395">
   <si>
     <t>Day</t>
   </si>
@@ -1374,6 +1374,22 @@
   </si>
   <si>
     <t>Algo(Stack / Queue Simulation )</t>
+  </si>
+  <si>
+    <t>Approach:
+Use two stacks — stack (all elements) and min_stack (tracks current min).
+Push to both when a new min appears; pop from both when min is removed.
+Pattern:
+Stack + Auxiliary Min Stack (Design Pattern).
+Complexity:
+Time: O(1) per operation
+Space: O(n)
+Notes:
+	•	Keeps constant-time getMin() lookup.
+	•	Common interview question testing stack-state tracking.</t>
+  </si>
+  <si>
+    <t>Algo(Stack / Design )</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2016,7 +2032,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2701,7 +2717,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2718,10 +2734,14 @@
         <v>241</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+        <v>394</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3">

</xml_diff>

<commit_message>
Day 25: Linked List Cycle - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B73B4F-7637-D749-828E-E4A899153877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAD0CF5-64D3-5642-950D-EC79311F7016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="397">
   <si>
     <t>Day</t>
   </si>
@@ -1390,6 +1390,22 @@
   </si>
   <si>
     <t>Algo(Stack / Design )</t>
+  </si>
+  <si>
+    <t>Approach:
+Use Floyd’s Cycle Detection (Tortoise &amp; Hare). Move one pointer 1 step and another 2 steps. If they meet → cycle exists.
+Pattern:
+Two Pointers / Fast-Slow Pointer Technique.
+Complexity:
+Time: O(n)
+Space: O(1)
+Notes:
+	•	Detects cycles efficiently without extra memory.
+	•	If no cycle, the fast pointer reaches None.
+	•	Related: Linked List Cycle II (find starting node of loop).</t>
+  </si>
+  <si>
+    <t>Algo(Linked List / Two Pointers  )</t>
   </si>
 </sst>
 </file>
@@ -1879,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2032,7 +2048,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2743,7 +2759,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2760,10 +2776,14 @@
         <v>242</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+        <v>396</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3">

</xml_diff>

<commit_message>
Day 26: Reverse Linked List - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAD0CF5-64D3-5642-950D-EC79311F7016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBF84E0-B0C5-9C48-824C-AE2F4EAC3C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="399">
   <si>
     <t>Day</t>
   </si>
@@ -1406,6 +1406,22 @@
   </si>
   <si>
     <t>Algo(Linked List / Two Pointers  )</t>
+  </si>
+  <si>
+    <t>Approach:
+Use two pointers (prev, curr). Iteratively reverse links: point curr.next to prev, then move both forward until list ends.
+Pattern:
+Linked List / Two-pointer manipulation.
+Complexity:
+Time: O(n)
+Space: O(1)
+Notes:
+	•	Key step: store next before reversing pointer.
+	•	Return prev (new head) at the end.
+	•	Recursive alternative exists but less memory-efficient.</t>
+  </si>
+  <si>
+    <t>Algo(Linked List / Iteration / Recursion)</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2048,7 +2064,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2785,7 +2801,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2802,10 +2818,14 @@
         <v>243</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+        <v>398</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
@@ -2826,7 +2846,9 @@
       <c r="F35" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -2848,7 +2870,9 @@
       <c r="F36" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -2870,7 +2894,9 @@
       <c r="F37" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -2914,7 +2940,9 @@
       <c r="F39" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -2936,7 +2964,9 @@
       <c r="F40" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -2958,7 +2988,9 @@
       <c r="F41" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Day 27: Rank Scores - SQL DENSE_RANK() solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBF84E0-B0C5-9C48-824C-AE2F4EAC3C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693FFF4D-144B-9D41-B6B9-AAB396AB51EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="401">
   <si>
     <t>Day</t>
   </si>
@@ -1422,6 +1422,23 @@
   </si>
   <si>
     <t>Algo(Linked List / Iteration / Recursion)</t>
+  </si>
+  <si>
+    <t>SQL / Window Functions / Ranking</t>
+  </si>
+  <si>
+    <t>Approach:
+Use the DENSE_RANK() window function to assign ranks based on scores in descending order. If multiple players share the same score, they get the same rank. The next distinct score gets the next consecutive rank number.
+Alternative (for older SQL versions): use a subquery to count distinct higher scores and add 1.
+Pattern:
+SQL Window Function — DENSE_RANK() for ranking without gaps.
+Complexity:
+	•	Time: O(N log N) due to sorting by score.
+	•	Space: O(1) additional memory.
+Notes:
+	•	DENSE_RANK() avoids gaps in ranking (unlike RANK()).
+	•	Must order by score DESC to rank highest first.
+	•	Alternative subquery approach works but is less efficient (O(N²)).</t>
   </si>
 </sst>
 </file>
@@ -1911,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2127,7 +2144,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -2827,7 +2844,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2844,12 +2861,14 @@
         <v>244</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>335</v>
+        <v>399</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="4" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3">

</xml_diff>

<commit_message>
Day 27: Duplicate Emails - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693FFF4D-144B-9D41-B6B9-AAB396AB51EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD7558-C3A9-6741-8B37-1031B4F7A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="401">
   <si>
     <t>Day</t>
   </si>
@@ -1928,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3031,7 +3031,9 @@
       <c r="F42" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Day 28: Merge Two Sorted Lists — solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B844F1-1691-8246-BB70-95F79829B2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8467ED7-A771-734D-AFF3-802E52D866E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="405">
   <si>
     <t>Day</t>
   </si>
@@ -1455,6 +1455,22 @@
   </si>
   <si>
     <t xml:space="preserve">SQL / Aggregation / Group By </t>
+  </si>
+  <si>
+    <t>Approach:
+Use a dummy node and two pointers to merge two sorted linked lists in one pass. Attach smaller nodes first and link remaining ones after one list ends.
+Pattern:
+Linked List Traversal / Two-Pointer Merge.
+Complexity:
+Time: O(m + n)
+Space: O(1)
+Notes:
+	•	Dummy node avoids extra conditions for head initialization.
+	•	Works even if one list is empty.
+	•	Same pattern used in Merge Sort merging step.</t>
+  </si>
+  <si>
+    <t>Algo(Linked List / Two Pointers)</t>
   </si>
 </sst>
 </file>
@@ -1944,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2097,7 +2113,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2912,7 +2928,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2929,12 +2945,14 @@
         <v>246</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>334</v>
+        <v>404</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="H37" s="4" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="3">

</xml_diff>

<commit_message>
Day 29: Palindrome Linked List - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8467ED7-A771-734D-AFF3-802E52D866E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F3D32C-396F-CF44-8728-03DC8876D35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="406">
   <si>
     <t>Day</t>
   </si>
@@ -1471,6 +1471,12 @@
   </si>
   <si>
     <t>Algo(Linked List / Two Pointers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Find middle with fast/slow; reverse the second half in-place; compare first half vs reversed second half; optionally restore.
+	•	Pattern: Two Pointers (fast/slow), In-place reverse, Half comparison.
+	•	Complexity: Time O(n), Space O(1).
+	•	Notes: For odd length, middle node is ignored during comparison; O(1) space avoids extra arrays/stacks; careful with pointer updates.</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="D38" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2113,7 +2119,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -2976,7 +2982,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2993,12 +2999,14 @@
         <v>247</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>334</v>
+        <v>404</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H39" s="3"/>
+      <c r="H39" s="4" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3">

</xml_diff>

<commit_message>
Day 30: Remove Nth Node From End of List - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F3D32C-396F-CF44-8728-03DC8876D35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0A1612-5C96-B44A-B9F1-C56EF7C0D9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="407">
   <si>
     <t>Day</t>
   </si>
@@ -1477,6 +1477,12 @@
 	•	Pattern: Two Pointers (fast/slow), In-place reverse, Half comparison.
 	•	Complexity: Time O(n), Space O(1).
 	•	Notes: For odd length, middle node is ignored during comparison; O(1) space avoids extra arrays/stacks; careful with pointer updates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Two-pointer technique with dummy node. Move fast n steps ahead, then move both until fast reaches end. Delete node after slow.
+	•	Pattern: Linked List, Two Pointers (fast/slow), Dummy Node.
+	•	Complexity: Time O(n), Space O(1).
+	•	Notes: Dummy node simplifies removing head; single-pass solution avoids counting list length; related to “Find Kth from End” pattern.</t>
   </si>
 </sst>
 </file>
@@ -1966,7 +1972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D38" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C39" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -2119,7 +2125,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -3008,7 +3014,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3025,12 +3031,14 @@
         <v>248</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>334</v>
+        <v>404</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="4" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3">

</xml_diff>

<commit_message>
Day 31: Design Linked List - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0A1612-5C96-B44A-B9F1-C56EF7C0D9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAC5CF6-4312-164C-8C30-C4C268DF9DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="409">
   <si>
     <t>Day</t>
   </si>
@@ -1483,6 +1483,15 @@
 	•	Pattern: Linked List, Two Pointers (fast/slow), Dummy Node.
 	•	Complexity: Time O(n), Space O(1).
 	•	Notes: Dummy node simplifies removing head; single-pass solution avoids counting list length; related to “Find Kth from End” pattern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Doubly linked list with head/tail sentinels; helpers for _get_node, _insert_before, _remove. Implement API: get, addAtHead, addAtTail, addAtIndex, deleteAtIndex.
+	•	Pattern: Linked List Design, Sentinels, Bidirectional traversal.
+	•	Complexity: get/addAtIndex/deleteAtIndex O(min(i, n−i)); addAtHead/addAtTail O(1). Space O(n).
+	•	Notes: Sentinels simplify edge cases; size tracking validates indexes; no built-in LinkedList used.</t>
+  </si>
+  <si>
+    <t>Algo(Linked List / Design)</t>
   </si>
 </sst>
 </file>
@@ -1972,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C39" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2125,7 +2134,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -3040,7 +3049,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3057,12 +3066,14 @@
         <v>249</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>334</v>
+        <v>408</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="4" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3">

</xml_diff>

<commit_message>
Day 32: LRU Cache - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAC5CF6-4312-164C-8C30-C4C268DF9DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1280D29-582A-9647-ADFB-D18E2AEA9497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="411">
   <si>
     <t>Day</t>
   </si>
@@ -1492,6 +1492,15 @@
   </si>
   <si>
     <t>Algo(Linked List / Design)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: HashMap (key → node) + Doubly Linked List with head/tail sentinels. On get/put, move node to head (MRU). On overflow, evict node before tail (LRU).
+	•	Pattern: Design; HashMap + Doubly Linked List; Recency tracking.
+	•	Complexity: Time O(1) for get/put; Space O(capacity).
+	•	Notes: Use sentinels to simplify inserts/removals; update existing keys in-place; eviction happens when size exceeds capacity.</t>
+  </si>
+  <si>
+    <t>Algo(Hashmap + Doubly Linked List (Design))</t>
   </si>
 </sst>
 </file>
@@ -1981,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="D41" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2134,7 +2143,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -3075,7 +3084,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3092,12 +3101,14 @@
         <v>250</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>334</v>
+        <v>410</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="4" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3">

</xml_diff>

<commit_message>
Day 33: Kth Largest Element in an Array - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1280D29-582A-9647-ADFB-D18E2AEA9497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B2DD91-8128-0D4E-9560-655CDDBB0BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="413">
   <si>
     <t>Day</t>
   </si>
@@ -1501,6 +1501,15 @@
   </si>
   <si>
     <t>Algo(Hashmap + Doubly Linked List (Design))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Use a Min-Heap of size k. For each number, push into heap and pop smallest if heap size &gt; k. The heap root gives the kth largest element.
+	•	Pattern: Heap / Priority Queue, Top K Elements.
+	•	Complexity: Time O(n log k); Space O(k).
+	•	Notes: Efficient for large arrays; avoids full sort. Quickselect offers O(n) average alternative but is harder to implement.</t>
+  </si>
+  <si>
+    <t>Algo(Heap / Quickselect )</t>
   </si>
 </sst>
 </file>
@@ -1990,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D41" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="D42" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2143,7 +2152,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -3110,7 +3119,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3127,10 +3136,14 @@
         <v>251</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+        <v>412</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="3">

</xml_diff>

<commit_message>
Day 34: Nth Highest Salary - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B2DD91-8128-0D4E-9560-655CDDBB0BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BDB26-1ACF-ED44-B44D-13BA590B4EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="415">
   <si>
     <t>Day</t>
   </si>
@@ -1510,6 +1510,23 @@
   </si>
   <si>
     <t>Algo(Heap / Quickselect )</t>
+  </si>
+  <si>
+    <t>Approach:
+Use the DENSE_RANK() window function to rank all distinct salaries in descending order. Then, select the salary where rnk = N. If there are fewer than N unique salaries, return NULL.
+Pattern:
+SQL Window Functions / Ranking Query.
+Complexity:
+Time: O(n log n) (ordering)
+Space: O(n).
+Notes:
+	•	DENSE_RANK() ensures ties get the same rank (unlike ROW_NUMBER() which counts duplicates separately).
+	•	Handles duplicates gracefully and avoids gaps between ranks.
+	•	Returns NULL automatically if no row matches the Nth rank.
+	•	Related to: Second Highest Salary (LeetCode 176) — this generalises it for any N.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL / Window Functions </t>
   </si>
 </sst>
 </file>
@@ -1999,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D42" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2215,7 +2232,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -3145,7 +3162,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="380" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3162,10 +3179,14 @@
         <v>252</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+        <v>414</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
@@ -3186,7 +3207,9 @@
       <c r="F45" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Day 34: Consecutive Numbers - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BDB26-1ACF-ED44-B44D-13BA590B4EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2365B92-D8CA-9F41-9A55-2E4020BCFB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="417">
   <si>
     <t>Day</t>
   </si>
@@ -1527,6 +1527,17 @@
   </si>
   <si>
     <t xml:space="preserve">SQL / Window Functions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach:
+	•	Self-join Logs on id+1 and id+2 where num matches across all three rows, then SELECT DISTINCT.
+	•	(Alt) MySQL 8+: LAG(num,1/2) over ORDER BY id and filter rows where all equal.
+	•	Pattern: Consecutive/streak detection; self-join or window LAG.
+	•	Complexity: ~O(n) scan with joins/window ops.
+	•	Notes: Self-join is portable to MySQL 5.x; window function is cleaner on MySQL 8+. Returns numbers with ≥3 consecutive occurrences.</t>
+  </si>
+  <si>
+    <t>SQL / Window / Self-Join</t>
   </si>
 </sst>
 </file>
@@ -2232,7 +2243,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -3188,7 +3199,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3205,12 +3216,14 @@
         <v>253</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>335</v>
+        <v>416</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="4" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="3">

</xml_diff>

<commit_message>
Day 34: Product Sales Analysis I - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2365B92-D8CA-9F41-9A55-2E4020BCFB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E64EA-C30D-FE46-BB28-FDB16C8E8121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="419">
   <si>
     <t>Day</t>
   </si>
@@ -1538,6 +1538,15 @@
   </si>
   <si>
     <t>SQL / Window / Self-Join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Perform an INNER JOIN between Sales and Product on product_id to fetch product_name, year, and price.
+	•	Pattern: SQL JOIN / Relational Mapping.
+	•	Complexity: O(n) join scan.
+	•	Notes: INNER JOIN filters out unsold products; use LEFT JOIN for full product list. Simple query demonstrating table relationships.</t>
+  </si>
+  <si>
+    <t>SQL / JOIN</t>
   </si>
 </sst>
 </file>
@@ -2027,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="D45" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2243,7 +2252,7 @@
       </c>
       <c r="J7" s="1">
         <f>COUNTIF(F2:F133,"SQL")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="335" x14ac:dyDescent="0.2">
@@ -3225,7 +3234,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3242,10 +3251,14 @@
         <v>254</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+        <v>418</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="3">

</xml_diff>

<commit_message>
Day 35: Binary Tree Inorder Traversal - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E64EA-C30D-FE46-BB28-FDB16C8E8121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE4ABD2-6969-334D-AFC3-5DAB0202F98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="421">
   <si>
     <t>Day</t>
   </si>
@@ -1547,6 +1547,15 @@
   </si>
   <si>
     <t>SQL / JOIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Inorder traversal (Left → Node → Right) using recursion; optional iterative version using stack to simulate recursion.
+	•	Pattern: DFS / Inorder Traversal.
+	•	Complexity: Time O(n), Space O(h).
+	•	Notes: Recursive is straightforward; iterative is more memory-efficient. Useful for BST validation and traversal-based problems.</t>
+  </si>
+  <si>
+    <t>Algo(Tree / DFS / Stack)</t>
   </si>
 </sst>
 </file>
@@ -2036,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D45" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2189,7 +2198,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -3260,7 +3269,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3277,10 +3286,14 @@
         <v>255</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+        <v>420</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="3">

</xml_diff>

<commit_message>
Day 36: Maximum Depth of Binary Tree - solution and notes
</commit_message>
<xml_diff>
--- a/leetcode_90days_tracker.xlsx
+++ b/leetcode_90days_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakthi/Library/CloudStorage/GoogleDrive-sakthibala7531@gmail.com/My Drive/Leetcode/leetcode-90days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE4ABD2-6969-334D-AFC3-5DAB0202F98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FB7F3C-D26F-3440-BAFB-5ABE5A16FE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="19240" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="423">
   <si>
     <t>Day</t>
   </si>
@@ -1556,6 +1556,15 @@
   </si>
   <si>
     <t>Algo(Tree / DFS / Stack)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	•	Approach: Recursive DFS → 1 + max(depth(left), depth(right)); optional BFS level-order for iterative version.
+	•	Pattern: Tree Traversal / DFS / BFS.
+	•	Complexity: Time O(n), Space O(h).
+	•	Notes: Recursion is cleanest; BFS is useful for understanding levels. Foundation for diameter and balance tree problems.</t>
+  </si>
+  <si>
+    <t>Algo(Tree / DFS / BFS)</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2055,7 @@
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2207,7 @@
       </c>
       <c r="J5" s="1">
         <f>COUNTIF(F2:F133,"Algo")</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="1">
         <f>COUNTIF(F2:F133,"Algo (Bonus)")</f>
@@ -3317,7 +3326,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3334,10 +3343,14 @@
         <v>256</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+        <v>422</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3">

</xml_diff>